<commit_message>
Branching works, need to add Shai and Tony stuff
</commit_message>
<xml_diff>
--- a/combined_results.xlsx
+++ b/combined_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,16 @@
           <t>Baricenter + Greedy Crossings</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>BranchAndReduce Duration [ns]</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>BranchAndReduce Crossings</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -476,7 +486,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7242</t>
+          <t>17658</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -486,7 +496,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>581</t>
+          <t>2041</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -496,7 +506,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>259</t>
+          <t>2800</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -506,10 +516,20 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>392</t>
+          <t>2001</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>14410</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -523,7 +543,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7207</t>
+          <t>19801</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -533,7 +553,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>442</t>
+          <t>2888</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -543,7 +563,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>208</t>
+          <t>1119</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -553,10 +573,20 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>311</t>
+          <t>3094</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>8152</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -570,7 +600,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1671956933</t>
+          <t>7286498594</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -580,7 +610,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4289</t>
+          <t>35228</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -590,7 +620,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>602</t>
+          <t>3201</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -600,10 +630,20 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>3652</t>
+          <t>33148</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>66427</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -617,7 +657,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5732</t>
+          <t>15386</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -627,7 +667,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>322</t>
+          <t>2794</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -637,7 +677,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>158</t>
+          <t>1099</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -647,10 +687,20 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>318</t>
+          <t>3043</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>8603</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -664,7 +714,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>26352</t>
+          <t>166373</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -674,7 +724,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>794</t>
+          <t>10707</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -684,7 +734,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>2920</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -694,10 +744,20 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>725</t>
+          <t>12638</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>23942</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>60</t>
         </is>
@@ -711,7 +771,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5157</t>
+          <t>15270</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -721,7 +781,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>225</t>
+          <t>2708</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -731,7 +791,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>995</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -741,10 +801,20 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>263</t>
+          <t>11964</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>11587</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -758,7 +828,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5925</t>
+          <t>17763</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -768,7 +838,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>711</t>
+          <t>3393</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -778,7 +848,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>269</t>
+          <t>1246</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -788,10 +858,20 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>647</t>
+          <t>3780</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>9698</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -805,7 +885,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5161</t>
+          <t>16871</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -815,7 +895,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>727</t>
+          <t>4863</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -825,7 +905,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>1246</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -835,10 +915,20 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>544</t>
+          <t>4822</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>11855</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -852,7 +942,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5034</t>
+          <t>13828</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -862,7 +952,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>226</t>
+          <t>2702</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -872,7 +962,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>1104</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -882,10 +972,20 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>245</t>
+          <t>2858</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>10542</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -899,7 +999,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1898882100</t>
+          <t>6106189208</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -909,7 +1009,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3010</t>
+          <t>27576</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -919,7 +1019,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>554</t>
+          <t>2919</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -929,10 +1029,20 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2906</t>
+          <t>28088</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>57681</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -946,7 +1056,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>118214</t>
+          <t>440286</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -956,7 +1066,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>480</t>
+          <t>5072</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -966,7 +1076,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>199</t>
+          <t>1234</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -976,10 +1086,20 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>582</t>
+          <t>5699</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>14609</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -993,7 +1113,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>169425</t>
+          <t>624144</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1003,7 +1123,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1694</t>
+          <t>7743</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1013,7 +1133,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>362</t>
+          <t>1697</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1023,10 +1143,20 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1731</t>
+          <t>7790</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>20513</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1040,7 +1170,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>26218</t>
+          <t>119308</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1050,7 +1180,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>823</t>
+          <t>6271</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1060,7 +1190,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>256</t>
+          <t>1664</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1070,12 +1200,22 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>717</t>
+          <t>17429</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
           <t>19</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>14656</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>17</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited performace.cpp to use median
</commit_message>
<xml_diff>
--- a/combined_results.xlsx
+++ b/combined_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,40 +439,30 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Greedy Duration [ns]</t>
+          <t>Barycenter Duration [ns]</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Greedy Crossings</t>
+          <t>Barycenter Crossings</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Baricenter Duration [ns]</t>
+          <t>Median Duration [ns]</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Baricenter Crossings</t>
+          <t>Median Crossings</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Baricenter + Greedy Duration [ns]</t>
+          <t>BranchAndReduce Duration [ns]</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>Baricenter + Greedy Crossings</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>BranchAndReduce Duration [ns]</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
         <is>
           <t>BranchAndReduce Crossings</t>
         </is>
@@ -486,7 +476,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>17658</t>
+          <t>2535</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -496,17 +486,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2041</t>
+          <t>532</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2800</t>
+          <t>416</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -516,20 +506,10 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2001</t>
+          <t>7725</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>14410</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -543,7 +523,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>19801</t>
+          <t>2536</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -553,7 +533,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2888</t>
+          <t>249</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -563,7 +543,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1119</t>
+          <t>449</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -573,20 +553,10 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>3094</t>
+          <t>18996</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>8152</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -600,7 +570,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>7286498594</t>
+          <t>383294106</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -610,40 +580,30 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>35228</t>
+          <t>696</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>13</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>3201</t>
+          <t>908</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>13</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>33148</t>
+          <t>23267</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>66427</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
         <is>
           <t>13</t>
         </is>
@@ -657,7 +617,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15386</t>
+          <t>3102</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -667,7 +627,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2794</t>
+          <t>184</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -677,7 +637,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1099</t>
+          <t>334</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -687,20 +647,10 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>3043</t>
+          <t>9256</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>8603</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -714,7 +664,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>166373</t>
+          <t>15397</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -724,7 +674,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>10707</t>
+          <t>311</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -734,7 +684,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2920</t>
+          <t>483</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -744,20 +694,10 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>12638</t>
+          <t>3497</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>23942</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
         <is>
           <t>60</t>
         </is>
@@ -771,7 +711,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15270</t>
+          <t>2704</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -781,17 +721,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2708</t>
+          <t>154</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>995</t>
+          <t>225</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -801,20 +741,10 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>11964</t>
+          <t>8480</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>11587</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -828,7 +758,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17763</t>
+          <t>4053</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -838,40 +768,30 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3393</t>
+          <t>243</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1246</t>
+          <t>413</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>3780</t>
+          <t>7139</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>9698</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -885,7 +805,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16871</t>
+          <t>3582</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -895,7 +815,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4863</t>
+          <t>245</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -905,7 +825,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1246</t>
+          <t>422</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -915,20 +835,10 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>4822</t>
+          <t>6033</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>11855</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
@@ -942,7 +852,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>13828</t>
+          <t>2781</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -952,17 +862,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2702</t>
+          <t>138</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>1104</t>
+          <t>282</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -972,20 +882,10 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2858</t>
+          <t>5123</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>10542</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -999,7 +899,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>6106189208</t>
+          <t>372812331</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1009,17 +909,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>27576</t>
+          <t>576</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2919</t>
+          <t>772</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1029,20 +929,10 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>28088</t>
+          <t>25228</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>57681</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
         <is>
           <t>17</t>
         </is>
@@ -1056,7 +946,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>440286</t>
+          <t>27331</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1066,17 +956,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>5072</t>
+          <t>217</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>293</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1086,20 +976,10 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>5699</t>
+          <t>7101</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>14609</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1113,7 +993,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>624144</t>
+          <t>59038</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1123,40 +1003,30 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>7743</t>
+          <t>373</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>1697</t>
+          <t>501</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>7790</t>
+          <t>6823</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>20513</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1170,7 +1040,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>119308</t>
+          <t>8429</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1180,40 +1050,30 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>6271</t>
+          <t>274</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>17</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1664</t>
+          <t>455</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>17429</t>
+          <t>9808</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>14656</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
         <is>
           <t>17</t>
         </is>

</xml_diff>